<commit_message>
sauvegade des fichiers excel
</commit_message>
<xml_diff>
--- a/uploadsLISTE.xlsx
+++ b/uploadsLISTE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9525" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9525" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -2239,8 +2239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2251,14 +2251,14 @@
     <col min="4" max="4" width="0.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>179</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" t="s">
         <v>180</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" t="s">
         <v>181</v>
       </c>
     </row>
@@ -2837,8 +2837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="K77" sqref="K77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3692,7 +3692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>

</xml_diff>